<commit_message>
working, but not friendly
all working for social network node and edge collection, but needs following quality of life improvements:
automating the generation of readable marriage ids
displaying names instead of uuid in relationships created from readable marriage id

next step: async variable designation for above issues.
</commit_message>
<xml_diff>
--- a/cohesionAndConflict_odkx/app/config/tables/families/forms/families/families.xlsx
+++ b/cohesionAndConflict_odkx/app/config/tables/families/forms/families/families.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-220" yWindow="1200" windowWidth="29980" windowHeight="16040" tabRatio="745" activeTab="6"/>
+    <workbookView xWindow="820" yWindow="180" windowWidth="32120" windowHeight="19060" tabRatio="745"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="7" r:id="rId1"/>
     <sheet name="survey" sheetId="1" r:id="rId2"/>
     <sheet name="choices" sheetId="3" r:id="rId3"/>
-    <sheet name="settings" sheetId="4" r:id="rId4"/>
-    <sheet name="model" sheetId="5" r:id="rId5"/>
+    <sheet name="model" sheetId="5" r:id="rId4"/>
+    <sheet name="settings" sheetId="4" r:id="rId5"/>
     <sheet name="family" sheetId="8" r:id="rId6"/>
     <sheet name="queries" sheetId="12" r:id="rId7"/>
   </sheets>
@@ -213,9 +213,6 @@
     <t>Parents:</t>
   </si>
   <si>
-    <t>Child</t>
-  </si>
-  <si>
     <t>Please enter info on child not living in household to the best of your ability</t>
   </si>
   <si>
@@ -238,6 +235,9 @@
   </si>
   <si>
     <t>used to add new members not living in household</t>
+  </si>
+  <si>
+    <t>Child:</t>
   </si>
 </sst>
 </file>
@@ -411,7 +411,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="163">
+  <cellStyleXfs count="165">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -501,6 +501,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -657,7 +659,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="163">
+  <cellStyles count="165">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -738,6 +740,7 @@
     <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -818,6 +821,7 @@
     <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="9"/>
     <cellStyle name="Note" xfId="88" builtinId="10"/>
@@ -1158,7 +1162,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1440,102 +1444,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="22.83203125" customWidth="1"/>
-    <col min="2" max="2" width="24.5" customWidth="1"/>
-    <col min="3" max="3" width="24.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A1" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="36" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A7" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C31"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1567,43 +1479,44 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>41</v>
-      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>49</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-    </row>
-    <row r="21" spans="2:3">
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-    </row>
-    <row r="24" spans="2:3">
-      <c r="B24" s="20"/>
-    </row>
-    <row r="26" spans="2:3">
-      <c r="B26" s="24"/>
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+    </row>
+    <row r="25" spans="2:3">
+      <c r="B25" s="20"/>
     </row>
     <row r="27" spans="2:3">
-      <c r="B27" s="26"/>
+      <c r="B27" s="24"/>
     </row>
     <row r="28" spans="2:3">
       <c r="B28" s="26"/>
@@ -1616,10 +1529,105 @@
     </row>
     <row r="31" spans="2:3">
       <c r="B31" s="26"/>
+    </row>
+    <row r="32" spans="2:3">
+      <c r="B32" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="22.83203125" customWidth="1"/>
+    <col min="2" max="2" width="24.5" customWidth="1"/>
+    <col min="3" max="3" width="24.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A1" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A8" s="3"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1633,7 +1641,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="G8" sqref="D8:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1674,7 +1682,7 @@
         <v>17</v>
       </c>
       <c r="J1" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -1764,7 +1772,7 @@
         <v>55</v>
       </c>
       <c r="G7" s="33" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="H7" s="33"/>
       <c r="I7" s="33"/>
@@ -1808,12 +1816,12 @@
       </c>
       <c r="F10" s="33"/>
       <c r="G10" s="33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H10" s="33"/>
       <c r="I10" s="33"/>
       <c r="J10" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1879,8 +1887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1963,7 +1971,7 @@
     </row>
     <row r="4" spans="1:9" ht="24">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
         <v>43</v>
@@ -1998,7 +2006,7 @@
     </row>
     <row r="6" spans="1:9" ht="24">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B6" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
Revert "Revert "Temp merge""
This reverts commit 6adb48ccc2ffb4eb9532e178a8a82c929325b6aa.
</commit_message>
<xml_diff>
--- a/cohesionAndConflict_odkx/app/config/tables/families/forms/families/families.xlsx
+++ b/cohesionAndConflict_odkx/app/config/tables/families/forms/families/families.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="180" windowWidth="32120" windowHeight="19060" tabRatio="745"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="745" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="7" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="settings" sheetId="4" r:id="rId5"/>
     <sheet name="family" sheetId="8" r:id="rId6"/>
     <sheet name="queries" sheetId="12" r:id="rId7"/>
+    <sheet name="prompt_types" sheetId="13" r:id="rId8"/>
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="100">
   <si>
     <t>type</t>
   </si>
@@ -238,13 +239,100 @@
   </si>
   <si>
     <t>Child:</t>
+  </si>
+  <si>
+    <t>marriage_id</t>
+  </si>
+  <si>
+    <t>readable</t>
+  </si>
+  <si>
+    <t>child_name</t>
+  </si>
+  <si>
+    <t>asyncs for child name and family id creation</t>
+  </si>
+  <si>
+    <t>async_assign_text_value</t>
+  </si>
+  <si>
+    <t>mariage id name</t>
+  </si>
+  <si>
+    <t>marriage_name_query</t>
+  </si>
+  <si>
+    <t>_id = ?</t>
+  </si>
+  <si>
+    <t>fieldname</t>
+  </si>
+  <si>
+    <t>uuid from linked table</t>
+  </si>
+  <si>
+    <t>marriage_name</t>
+  </si>
+  <si>
+    <t>isSessionVariable</t>
+  </si>
+  <si>
+    <t>display.debug</t>
+  </si>
+  <si>
+    <t>prompt_type_name</t>
+  </si>
+  <si>
+    <t>async_assign_count</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>async_assign_num_value</t>
+  </si>
+  <si>
+    <t>marr name :: {{data.marriage_name}}</t>
+  </si>
+  <si>
+    <t>child_name_query</t>
+  </si>
+  <si>
+    <t>[ data('child') ]</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>child name :: {{data.child_name}}</t>
+  </si>
+  <si>
+    <t>child_id :: {{data.child}}</t>
+  </si>
+  <si>
+    <t>marriage_uuid</t>
+  </si>
+  <si>
+    <t>[ data('marriage_uuid') ]</t>
+  </si>
+  <si>
+    <t>marr_id :: {{data.marriage_uuid}}</t>
+  </si>
+  <si>
+    <t>assign</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>data('marriage_name') + "=" + data('child_name')</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -278,6 +366,21 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -411,7 +514,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="165">
+  <cellStyleXfs count="178">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -577,8 +680,21 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -658,8 +774,15 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="169" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="169" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="169" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="165">
+  <cellStyles count="178">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -741,6 +864,12 @@
     <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="171" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="173" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="175" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="177" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -822,8 +951,15 @@
     <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="170" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="172" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="174" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="176" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="9"/>
+    <cellStyle name="Normal 4" xfId="169"/>
     <cellStyle name="Note" xfId="88" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1162,7 +1298,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1215,7 +1351,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1444,10 +1580,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1459,7 +1595,7 @@
     <col min="5" max="5" width="46.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="12.75" customHeight="1">
+    <row r="1" spans="1:4" ht="12.75" customHeight="1">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -1469,69 +1605,103 @@
       <c r="C1" s="9" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="12.75" customHeight="1">
+      <c r="D1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="12.75" customHeight="1">
       <c r="B2" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-    </row>
-    <row r="4" spans="1:3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="12.75" customHeight="1">
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" s="10" t="s">
+      <c r="B8" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-    </row>
-    <row r="22" spans="2:3">
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
+      <c r="C8" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="B9" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="B10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="25" spans="2:3">
-      <c r="B25" s="20"/>
-    </row>
-    <row r="27" spans="2:3">
-      <c r="B27" s="24"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
     </row>
     <row r="28" spans="2:3">
-      <c r="B28" s="26"/>
-    </row>
-    <row r="29" spans="2:3">
-      <c r="B29" s="26"/>
+      <c r="B28" s="20"/>
     </row>
     <row r="30" spans="2:3">
-      <c r="B30" s="26"/>
+      <c r="B30" s="24"/>
     </row>
     <row r="31" spans="2:3">
       <c r="B31" s="26"/>
     </row>
     <row r="32" spans="2:3">
       <c r="B32" s="26"/>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" s="26"/>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" s="26"/>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1549,7 +1719,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1638,22 +1808,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="D8:G8"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="3" max="3" width="25.6640625" customWidth="1"/>
-    <col min="4" max="4" width="18.5" customWidth="1"/>
+    <col min="4" max="4" width="22.1640625" customWidth="1"/>
+    <col min="5" max="5" width="18.1640625" customWidth="1"/>
     <col min="7" max="7" width="48.6640625" customWidth="1"/>
     <col min="10" max="10" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="31" customHeight="1">
+    <row r="1" spans="1:11" ht="31" customHeight="1">
       <c r="A1" s="16" t="s">
         <v>28</v>
       </c>
@@ -1684,8 +1855,11 @@
       <c r="J1" s="18" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="30"/>
       <c r="B2" s="30" t="s">
         <v>29</v>
@@ -1698,7 +1872,7 @@
       <c r="H2" s="31"/>
       <c r="I2" s="31"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11">
       <c r="A3" s="32"/>
       <c r="B3" s="32"/>
       <c r="C3" s="32"/>
@@ -1713,7 +1887,7 @@
       <c r="H3" s="33"/>
       <c r="I3" s="33"/>
     </row>
-    <row r="4" spans="1:10" ht="52" customHeight="1">
+    <row r="4" spans="1:11" ht="52" customHeight="1">
       <c r="A4" s="32"/>
       <c r="B4" s="32"/>
       <c r="C4" s="32"/>
@@ -1728,7 +1902,7 @@
       <c r="H4" s="33"/>
       <c r="I4" s="33"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:11">
       <c r="A5" s="32"/>
       <c r="B5" s="32"/>
       <c r="C5" s="32"/>
@@ -1739,7 +1913,7 @@
         <v>58</v>
       </c>
       <c r="F5" s="32" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="G5" s="32" t="s">
         <v>61</v>
@@ -1747,7 +1921,7 @@
       <c r="H5" s="33"/>
       <c r="I5" s="33"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11">
       <c r="A6" s="32"/>
       <c r="B6" s="32"/>
       <c r="C6" s="32"/>
@@ -1758,7 +1932,7 @@
       <c r="H6" s="33"/>
       <c r="I6" s="33"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:11">
       <c r="A7" s="32"/>
       <c r="B7" s="32"/>
       <c r="C7" s="32"/>
@@ -1777,7 +1951,7 @@
       <c r="H7" s="33"/>
       <c r="I7" s="33"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:11">
       <c r="A8" s="33"/>
       <c r="B8" s="33"/>
       <c r="C8" s="33"/>
@@ -1788,7 +1962,7 @@
       <c r="H8" s="33"/>
       <c r="I8" s="33"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:11">
       <c r="A9" s="33"/>
       <c r="B9" s="33"/>
       <c r="C9" s="33"/>
@@ -1804,7 +1978,7 @@
       <c r="I9" s="33"/>
       <c r="J9" s="20"/>
     </row>
-    <row r="10" spans="1:10" ht="24">
+    <row r="10" spans="1:11" ht="24">
       <c r="A10" s="33"/>
       <c r="B10" s="33"/>
       <c r="C10" s="33"/>
@@ -1824,7 +1998,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:11">
       <c r="A11" s="28"/>
       <c r="B11" s="28"/>
       <c r="C11" s="28"/>
@@ -1836,7 +2010,7 @@
       <c r="I11" s="28"/>
       <c r="J11" s="20"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:11">
       <c r="A12" s="31"/>
       <c r="B12" s="31" t="s">
         <v>30</v>
@@ -1849,7 +2023,7 @@
       <c r="H12" s="31"/>
       <c r="I12" s="31"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:11">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -1858,19 +2032,113 @@
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:11">
       <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
+      <c r="B14" s="10" t="s">
+        <v>29</v>
+      </c>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
     </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="10"/>
+    <row r="15" spans="1:11" ht="24">
+      <c r="A15" t="s">
+        <v>74</v>
+      </c>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
+      <c r="D15" t="s">
+        <v>75</v>
+      </c>
+      <c r="E15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" t="s">
+        <v>81</v>
+      </c>
+      <c r="K15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" t="s">
+        <v>89</v>
+      </c>
+      <c r="F16" t="s">
+        <v>73</v>
+      </c>
+      <c r="K16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9">
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+    </row>
+    <row r="18" spans="2:9">
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9">
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9">
+      <c r="D20" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9">
+      <c r="D21" t="s">
+        <v>18</v>
+      </c>
+      <c r="G21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9">
+      <c r="D22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G22" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9">
+      <c r="D23" t="s">
+        <v>18</v>
+      </c>
+      <c r="G23" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9">
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" ht="36">
+      <c r="D25" t="s">
+        <v>97</v>
+      </c>
+      <c r="F25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I25" t="s">
+        <v>99</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1885,10 +2153,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1903,7 +2171,7 @@
     <col min="9" max="9" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="23" customFormat="1">
+    <row r="1" spans="1:10" s="23" customFormat="1">
       <c r="A1" s="19" t="s">
         <v>22</v>
       </c>
@@ -1931,8 +2199,11 @@
       <c r="I1" s="23" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="D2" s="24"/>
       <c r="E2" s="24"/>
       <c r="F2" s="24"/>
@@ -1940,7 +2211,7 @@
       <c r="H2" s="24"/>
       <c r="I2" s="24"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>57</v>
       </c>
@@ -1969,7 +2240,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="24">
+    <row r="4" spans="1:10" ht="24">
       <c r="A4" t="s">
         <v>68</v>
       </c>
@@ -1998,13 +2269,13 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="F5" s="24"/>
       <c r="G5" s="24"/>
       <c r="H5" s="24"/>
       <c r="I5" s="24"/>
     </row>
-    <row r="6" spans="1:9" ht="24">
+    <row r="6" spans="1:10" ht="24">
       <c r="A6" t="s">
         <v>69</v>
       </c>
@@ -2033,7 +2304,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="15" customFormat="1">
+    <row r="8" spans="1:10" s="15" customFormat="1">
       <c r="B8" s="25"/>
       <c r="C8" s="25"/>
       <c r="D8" s="25"/>
@@ -2043,18 +2314,66 @@
       <c r="H8" s="25"/>
       <c r="I8" s="25"/>
     </row>
-    <row r="9" spans="1:9">
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="24"/>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="I10" s="24"/>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="G9" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="H9" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="I9" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="J9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="B10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" t="s">
+        <v>78</v>
+      </c>
+      <c r="G10" t="s">
+        <v>90</v>
+      </c>
+      <c r="H10" t="s">
+        <v>48</v>
+      </c>
+      <c r="I10" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="J10" t="s">
+        <v>91</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2065,4 +2384,63 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="14">
+      <c r="A2" s="37"/>
+      <c r="B2" s="37"/>
+    </row>
+    <row r="3" spans="1:2" ht="14">
+      <c r="A3" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="14">
+      <c r="A4" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" s="39" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14">
+      <c r="A5" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
UX improvements for families and marriages
</commit_message>
<xml_diff>
--- a/cohesionAndConflict_odkx/app/config/tables/families/forms/families/families.xlsx
+++ b/cohesionAndConflict_odkx/app/config/tables/families/forms/families/families.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="745" activeTab="3"/>
+    <workbookView xWindow="1200" yWindow="80" windowWidth="30520" windowHeight="18740" tabRatio="745" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="7" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="99">
   <si>
     <t>type</t>
   </si>
@@ -193,9 +193,6 @@
     <t>family_id</t>
   </si>
   <si>
-    <t>child</t>
-  </si>
-  <si>
     <t>do section family</t>
   </si>
   <si>
@@ -265,9 +262,6 @@
     <t>_id = ?</t>
   </si>
   <si>
-    <t>fieldname</t>
-  </si>
-  <si>
     <t>uuid from linked table</t>
   </si>
   <si>
@@ -298,27 +292,12 @@
     <t>child_name_query</t>
   </si>
   <si>
-    <t>[ data('child') ]</t>
-  </si>
-  <si>
     <t>first_name</t>
   </si>
   <si>
     <t>child name :: {{data.child_name}}</t>
   </si>
   <si>
-    <t>child_id :: {{data.child}}</t>
-  </si>
-  <si>
-    <t>marriage_uuid</t>
-  </si>
-  <si>
-    <t>[ data('marriage_uuid') ]</t>
-  </si>
-  <si>
-    <t>marr_id :: {{data.marriage_uuid}}</t>
-  </si>
-  <si>
     <t>assign</t>
   </si>
   <si>
@@ -326,6 +305,24 @@
   </si>
   <si>
     <t>data('marriage_name') + "=" + data('child_name')</t>
+  </si>
+  <si>
+    <t>child_id</t>
+  </si>
+  <si>
+    <t>child_id :: {{data.child_id}}</t>
+  </si>
+  <si>
+    <t>marr_id :: {{data.marriage_id}}</t>
+  </si>
+  <si>
+    <t>fieldName</t>
+  </si>
+  <si>
+    <t>[ data('marriage_id') ]</t>
+  </si>
+  <si>
+    <t>[ data('child_id') ]</t>
   </si>
 </sst>
 </file>
@@ -1401,7 +1398,7 @@
     <row r="2" spans="1:10" ht="36.75" customHeight="1">
       <c r="A2" s="10"/>
       <c r="B2" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
@@ -1582,8 +1579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1606,7 +1603,7 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="12.75" customHeight="1">
@@ -1614,7 +1611,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="12.75" customHeight="1">
@@ -1623,13 +1620,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>98</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1638,13 +1635,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>54</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1656,7 +1653,7 @@
         <v>49</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>55</v>
+        <v>93</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>14</v>
@@ -1664,18 +1661,18 @@
     </row>
     <row r="9" spans="1:4">
       <c r="B9" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="B10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="2:3">
@@ -1745,7 +1742,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="18.75" customHeight="1">
@@ -1761,7 +1758,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="12.75" customHeight="1">
@@ -1778,16 +1775,16 @@
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="18.75" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="18.75" customHeight="1">
@@ -1811,7 +1808,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1853,10 +1850,10 @@
         <v>17</v>
       </c>
       <c r="J1" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -1882,7 +1879,7 @@
       <c r="E3" s="32"/>
       <c r="F3" s="32"/>
       <c r="G3" s="32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H3" s="33"/>
       <c r="I3" s="33"/>
@@ -1897,7 +1894,7 @@
       <c r="E4" s="32"/>
       <c r="F4" s="32"/>
       <c r="G4" s="33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H4" s="33"/>
       <c r="I4" s="33"/>
@@ -1910,13 +1907,13 @@
         <v>14</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F5" s="32" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="G5" s="32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H5" s="33"/>
       <c r="I5" s="33"/>
@@ -1943,10 +1940,10 @@
         <v>43</v>
       </c>
       <c r="F7" s="33" t="s">
-        <v>55</v>
+        <v>93</v>
       </c>
       <c r="G7" s="33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H7" s="33"/>
       <c r="I7" s="33"/>
@@ -1990,12 +1987,12 @@
       </c>
       <c r="F10" s="33"/>
       <c r="G10" s="33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H10" s="33"/>
       <c r="I10" s="33"/>
       <c r="J10" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -2045,18 +2042,18 @@
     </row>
     <row r="15" spans="1:11" ht="24">
       <c r="A15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
       <c r="D15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K15" t="b">
         <v>1</v>
@@ -2066,13 +2063,13 @@
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E16" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K16" t="b">
         <v>1</v>
@@ -2097,7 +2094,7 @@
         <v>18</v>
       </c>
       <c r="G20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="2:9">
@@ -2105,7 +2102,7 @@
         <v>18</v>
       </c>
       <c r="G21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="2:9">
@@ -2113,7 +2110,7 @@
         <v>18</v>
       </c>
       <c r="G22" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="2:9">
@@ -2121,7 +2118,7 @@
         <v>18</v>
       </c>
       <c r="G23" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="2:9">
@@ -2131,13 +2128,13 @@
     </row>
     <row r="25" spans="2:9" ht="36">
       <c r="D25" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="F25" t="s">
         <v>54</v>
       </c>
       <c r="I25" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -2155,8 +2152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2200,7 +2197,7 @@
         <v>40</v>
       </c>
       <c r="J1" s="23" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -2213,10 +2210,10 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
         <v>57</v>
-      </c>
-      <c r="B3" t="s">
-        <v>58</v>
       </c>
       <c r="C3" t="s">
         <v>44</v>
@@ -2242,7 +2239,7 @@
     </row>
     <row r="4" spans="1:10" ht="24">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
         <v>43</v>
@@ -2277,7 +2274,7 @@
     </row>
     <row r="6" spans="1:10" ht="24">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B6" t="s">
         <v>50</v>
@@ -2316,10 +2313,10 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" t="s">
         <v>76</v>
-      </c>
-      <c r="B9" t="s">
-        <v>77</v>
       </c>
       <c r="C9" t="s">
         <v>44</v>
@@ -2331,10 +2328,10 @@
         <v>42</v>
       </c>
       <c r="F9" s="24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G9" s="24" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="H9" s="24" t="s">
         <v>48</v>
@@ -2343,12 +2340,12 @@
         <v>48</v>
       </c>
       <c r="J9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="B10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C10" t="s">
         <v>44</v>
@@ -2360,10 +2357,10 @@
         <v>8</v>
       </c>
       <c r="F10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G10" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="H10" t="s">
         <v>48</v>
@@ -2372,7 +2369,7 @@
         <v>48</v>
       </c>
       <c r="J10" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -2401,7 +2398,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="36" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B1" s="36" t="s">
         <v>0</v>
@@ -2413,23 +2410,23 @@
     </row>
     <row r="3" spans="1:2" ht="14">
       <c r="A3" s="38" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14">
       <c r="A4" s="39" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B4" s="39" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="14">
       <c r="A5" s="39" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5" s="39" t="s">
         <v>41</v>

</xml_diff>